<commit_message>
added multi pie chart section
</commit_message>
<xml_diff>
--- a/.data/burrito/burrito_pie_chart.xlsx
+++ b/.data/burrito/burrito_pie_chart.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jji/Projects/hotplots.science/_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jji/Projects/hotplots/.data/burrito/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2016" sheetId="1" r:id="rId1"/>
+    <sheet name="2003" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Chipotle</t>
   </si>
@@ -45,6 +46,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -74,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,7 +177,7 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:doughnutChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
@@ -299,7 +304,6 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="1"/>
@@ -328,7 +332,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>'2016'!$A$1:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -348,7 +352,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>'2016'!$B$1:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -369,7 +373,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="1"/>
@@ -379,7 +382,8 @@
           <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -475,6 +479,330 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2003'!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Chipotle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Qdoba</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Local Chain</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Taco Bell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2003'!$B$1:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -518,6 +846,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
@@ -1119,20 +1487,621 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1151,7 +2120,185 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02662</cdr:x>
+      <cdr:y>0.39919</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.20152</cdr:x>
+      <cdr:y>0.60484</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="177800" y="1257300"/>
+          <a:ext cx="1168400" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="3200"/>
+            <a:t>2016</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02662</cdr:x>
+      <cdr:y>0.30769</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.20152</cdr:x>
+      <cdr:y>0.58791</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="177800" y="711200"/>
+          <a:ext cx="1168400" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="3200"/>
+            <a:t>2003</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1417,10 +2564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,8 +2604,58 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>